<commit_message>
updated UI for batch operation
</commit_message>
<xml_diff>
--- a/sitedb/smallcell data/activation table.xlsx
+++ b/sitedb/smallcell data/activation table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python Project\005 VHA Macro site workflow\Django-Workflow\sitedb\smallcell data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08438E5B-305E-48C9-AC29-A4CD8D890A27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA80A67C-48E5-406B-90EC-674FD1719DA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{99F59DCC-3D2B-46F9-9A8F-32B40955F386}"/>
+    <workbookView xWindow="28680" yWindow="-6645" windowWidth="29040" windowHeight="15840" xr2:uid="{99F59DCC-3D2B-46F9-9A8F-32B40955F386}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1563,7 +1563,7 @@
     <t>Activation Status</t>
   </si>
   <si>
-    <t>Not Started</t>
+    <t>not_started</t>
   </si>
 </sst>
 </file>
@@ -1971,7 +1971,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACF5D73B-F7AF-41B4-882A-974DF290516B}">
   <dimension ref="A1:C496"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>